<commit_message>
entregables mas o menos corregidos
</commit_message>
<xml_diff>
--- a/Entregables/Informe de avance/Informe de Avance - Periodo 1.xlsx
+++ b/Entregables/Informe de avance/Informe de Avance - Periodo 1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuliano\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -332,12 +332,6 @@
     <t>Utilizamos menos costos para la actividad que realizamos</t>
   </si>
   <si>
-    <t>Lo que falta para terminar el proyecto según lo presupuestado</t>
-  </si>
-  <si>
-    <t>Lo que falta para terminar el proyecto si seguimos así</t>
-  </si>
-  <si>
     <t>Lo que va a costar el proyecto según lo presupuestado</t>
   </si>
   <si>
@@ -397,6 +391,12 @@
       </rPr>
       <t xml:space="preserve"> Al planificar el primer período con la mitad de la actividad de diseño de base de datos, fue fácil cumplir con el objetivo, obteniendo un SPI de 1. Una estimación perfecta en base al calendario pero nos sobrepasamos por dos horas del costo estimado.</t>
     </r>
+  </si>
+  <si>
+    <t>Horas que faltan para terminar el proyecto según lo presupuestado</t>
+  </si>
+  <si>
+    <t>Horas que faltan para terminar el proyecto si seguimos de esta manera</t>
   </si>
 </sst>
 </file>
@@ -1490,6 +1490,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1594,7 +1595,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2425,46 +2425,46 @@
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="83"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="85" t="s">
+      <c r="C1" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="84"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="83"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="82" t="s">
+      <c r="G1" s="84"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="83"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="85" t="s">
+      <c r="J1" s="84"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="83"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="90" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="87" t="s">
+      <c r="M1" s="84"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="88"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="87" t="s">
+      <c r="S1" s="89"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="88"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="82" t="s">
+      <c r="V1" s="89"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="85"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -4433,8 +4433,8 @@
       <c r="A45" s="72"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="130" t="s">
-        <v>113</v>
+      <c r="A46" s="82" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5734,8 +5734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49:K51"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43:K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5750,29 +5750,29 @@
   <sheetData>
     <row r="1" spans="1:26" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="112" t="s">
+      <c r="B2" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="114"/>
+      <c r="J2" s="114"/>
+      <c r="K2" s="115"/>
     </row>
     <row r="4" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="115" t="s">
+      <c r="C4" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="118"/>
       <c r="I4" s="44"/>
       <c r="J4" s="44"/>
     </row>
@@ -5780,23 +5780,23 @@
       <c r="B5" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="94">
+      <c r="C5" s="95">
         <v>43735</v>
       </c>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="97"/>
     </row>
     <row r="6" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="C6" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="94"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="47"/>
@@ -6052,18 +6052,18 @@
     </row>
     <row r="22" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
-      <c r="B22" s="97" t="s">
-        <v>114</v>
-      </c>
-      <c r="C22" s="98"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
-      <c r="I22" s="98"/>
-      <c r="J22" s="98"/>
-      <c r="K22" s="99"/>
+      <c r="B22" s="98" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="99"/>
+      <c r="J22" s="99"/>
+      <c r="K22" s="100"/>
       <c r="L22" s="49"/>
       <c r="M22" s="49"/>
       <c r="N22" s="49"/>
@@ -6082,16 +6082,16 @@
     </row>
     <row r="23" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="49"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="101"/>
-      <c r="I23" s="101"/>
-      <c r="J23" s="101"/>
-      <c r="K23" s="102"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="102"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="102"/>
+      <c r="I23" s="102"/>
+      <c r="J23" s="102"/>
+      <c r="K23" s="103"/>
       <c r="L23" s="49"/>
       <c r="M23" s="49"/>
       <c r="N23" s="49"/>
@@ -6110,16 +6110,16 @@
     </row>
     <row r="24" spans="1:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="49"/>
-      <c r="B24" s="103"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
-      <c r="E24" s="104"/>
-      <c r="F24" s="104"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="104"/>
-      <c r="I24" s="104"/>
-      <c r="J24" s="104"/>
-      <c r="K24" s="105"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="105"/>
+      <c r="J24" s="105"/>
+      <c r="K24" s="106"/>
       <c r="L24" s="49"/>
       <c r="M24" s="49"/>
       <c r="N24" s="49"/>
@@ -6166,40 +6166,40 @@
     </row>
     <row r="26" spans="1:26" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="106" t="s">
+      <c r="B27" s="107" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="107"/>
-      <c r="D27" s="107"/>
-      <c r="E27" s="107"/>
-      <c r="F27" s="107"/>
-      <c r="G27" s="107"/>
-      <c r="H27" s="107"/>
-      <c r="I27" s="107"/>
-      <c r="J27" s="107"/>
-      <c r="K27" s="108"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="109"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="109" t="s">
+      <c r="B32" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="110"/>
-      <c r="D32" s="109" t="s">
+      <c r="C32" s="111"/>
+      <c r="D32" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="110"/>
-      <c r="F32" s="109" t="s">
+      <c r="E32" s="111"/>
+      <c r="F32" s="110" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="111"/>
-      <c r="H32" s="111"/>
-      <c r="I32" s="111"/>
-      <c r="J32" s="111"/>
-      <c r="K32" s="110"/>
+      <c r="G32" s="112"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="112"/>
+      <c r="K32" s="111"/>
     </row>
     <row r="33" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="52" t="s">
@@ -6209,14 +6209,14 @@
         <f>+Cálculos!B48</f>
         <v>213</v>
       </c>
-      <c r="D33" s="121"/>
-      <c r="E33" s="122"/>
-      <c r="F33" s="127"/>
-      <c r="G33" s="122"/>
-      <c r="H33" s="122"/>
-      <c r="I33" s="122"/>
-      <c r="J33" s="122"/>
-      <c r="K33" s="128"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="123"/>
+      <c r="F33" s="128"/>
+      <c r="G33" s="123"/>
+      <c r="H33" s="123"/>
+      <c r="I33" s="123"/>
+      <c r="J33" s="123"/>
+      <c r="K33" s="129"/>
     </row>
     <row r="34" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="58" t="s">
@@ -6226,16 +6226,16 @@
         <f>+Cálculos!B52</f>
         <v>4</v>
       </c>
-      <c r="D34" s="118"/>
-      <c r="E34" s="95"/>
-      <c r="F34" s="119" t="s">
-        <v>106</v>
-      </c>
-      <c r="G34" s="95"/>
-      <c r="H34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="J34" s="95"/>
-      <c r="K34" s="96"/>
+      <c r="D34" s="119"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="120" t="s">
+        <v>104</v>
+      </c>
+      <c r="G34" s="96"/>
+      <c r="H34" s="96"/>
+      <c r="I34" s="96"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="97"/>
     </row>
     <row r="35" spans="2:11" s="78" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="81" t="s">
@@ -6248,7 +6248,7 @@
       <c r="D35" s="79"/>
       <c r="E35" s="76"/>
       <c r="F35" s="80" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G35" s="76"/>
       <c r="H35" s="76"/>
@@ -6264,16 +6264,16 @@
         <f>+Cálculos!B54</f>
         <v>2</v>
       </c>
-      <c r="D36" s="118"/>
-      <c r="E36" s="95"/>
-      <c r="F36" s="119" t="s">
-        <v>107</v>
-      </c>
-      <c r="G36" s="95"/>
-      <c r="H36" s="95"/>
-      <c r="I36" s="95"/>
-      <c r="J36" s="95"/>
-      <c r="K36" s="96"/>
+      <c r="D36" s="119"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="120" t="s">
+        <v>105</v>
+      </c>
+      <c r="G36" s="96"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="96"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="97"/>
     </row>
     <row r="37" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="52" t="s">
@@ -6283,18 +6283,18 @@
         <f>+Cálculos!E52</f>
         <v>0</v>
       </c>
-      <c r="D37" s="118" t="s">
+      <c r="D37" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="E37" s="95"/>
-      <c r="F37" s="129" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="95"/>
-      <c r="H37" s="95"/>
-      <c r="I37" s="95"/>
-      <c r="J37" s="95"/>
-      <c r="K37" s="96"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="130" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="96"/>
+      <c r="H37" s="96"/>
+      <c r="I37" s="96"/>
+      <c r="J37" s="96"/>
+      <c r="K37" s="97"/>
     </row>
     <row r="38" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="58" t="s">
@@ -6304,18 +6304,18 @@
         <f>+Cálculos!E53</f>
         <v>2</v>
       </c>
-      <c r="D38" s="118" t="s">
+      <c r="D38" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="95"/>
-      <c r="F38" s="119" t="s">
-        <v>110</v>
-      </c>
-      <c r="G38" s="95"/>
-      <c r="H38" s="95"/>
-      <c r="I38" s="95"/>
-      <c r="J38" s="95"/>
-      <c r="K38" s="96"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="120" t="s">
+        <v>108</v>
+      </c>
+      <c r="G38" s="96"/>
+      <c r="H38" s="96"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="96"/>
+      <c r="K38" s="97"/>
     </row>
     <row r="39" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="58" t="s">
@@ -6325,18 +6325,18 @@
         <f>+Cálculos!E54</f>
         <v>1</v>
       </c>
-      <c r="D39" s="118" t="s">
+      <c r="D39" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="E39" s="95"/>
-      <c r="F39" s="119" t="s">
-        <v>111</v>
-      </c>
-      <c r="G39" s="95"/>
-      <c r="H39" s="95"/>
-      <c r="I39" s="95"/>
-      <c r="J39" s="95"/>
-      <c r="K39" s="96"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="120" t="s">
+        <v>109</v>
+      </c>
+      <c r="G39" s="96"/>
+      <c r="H39" s="96"/>
+      <c r="I39" s="96"/>
+      <c r="J39" s="96"/>
+      <c r="K39" s="97"/>
     </row>
     <row r="40" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="58" t="s">
@@ -6346,18 +6346,18 @@
         <f>+Cálculos!E55</f>
         <v>2</v>
       </c>
-      <c r="D40" s="118" t="s">
+      <c r="D40" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="E40" s="95"/>
-      <c r="F40" s="119" t="s">
+      <c r="E40" s="96"/>
+      <c r="F40" s="120" t="s">
         <v>100</v>
       </c>
-      <c r="G40" s="95"/>
-      <c r="H40" s="95"/>
-      <c r="I40" s="95"/>
-      <c r="J40" s="95"/>
-      <c r="K40" s="96"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="96"/>
+      <c r="J40" s="96"/>
+      <c r="K40" s="97"/>
     </row>
     <row r="41" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="58" t="s">
@@ -6367,18 +6367,18 @@
         <f>+Cálculos!E56</f>
         <v>209</v>
       </c>
-      <c r="D41" s="118" t="s">
+      <c r="D41" s="119" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="95"/>
-      <c r="F41" s="119" t="s">
-        <v>101</v>
-      </c>
-      <c r="G41" s="95"/>
-      <c r="H41" s="95"/>
-      <c r="I41" s="95"/>
-      <c r="J41" s="95"/>
-      <c r="K41" s="96"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="120" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="96"/>
+      <c r="H41" s="96"/>
+      <c r="I41" s="96"/>
+      <c r="J41" s="96"/>
+      <c r="K41" s="97"/>
     </row>
     <row r="42" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="58" t="s">
@@ -6388,18 +6388,18 @@
         <f>+Cálculos!E57</f>
         <v>104.5</v>
       </c>
-      <c r="D42" s="118" t="s">
+      <c r="D42" s="119" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="95"/>
-      <c r="F42" s="119" t="s">
-        <v>102</v>
-      </c>
-      <c r="G42" s="95"/>
-      <c r="H42" s="95"/>
-      <c r="I42" s="95"/>
-      <c r="J42" s="95"/>
-      <c r="K42" s="96"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="120" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" s="96"/>
+      <c r="H42" s="96"/>
+      <c r="I42" s="96"/>
+      <c r="J42" s="96"/>
+      <c r="K42" s="97"/>
     </row>
     <row r="43" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="58" t="s">
@@ -6409,18 +6409,18 @@
         <f>+Cálculos!E58</f>
         <v>213</v>
       </c>
-      <c r="D43" s="118" t="s">
+      <c r="D43" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="95"/>
-      <c r="F43" s="119" t="s">
-        <v>103</v>
-      </c>
-      <c r="G43" s="95"/>
-      <c r="H43" s="95"/>
-      <c r="I43" s="95"/>
-      <c r="J43" s="95"/>
-      <c r="K43" s="96"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="120" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43" s="96"/>
+      <c r="H43" s="96"/>
+      <c r="I43" s="96"/>
+      <c r="J43" s="96"/>
+      <c r="K43" s="97"/>
     </row>
     <row r="44" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="58" t="s">
@@ -6430,18 +6430,18 @@
         <f>+Cálculos!E59</f>
         <v>106.5</v>
       </c>
-      <c r="D44" s="118" t="s">
+      <c r="D44" s="119" t="s">
         <v>69</v>
       </c>
-      <c r="E44" s="95"/>
-      <c r="F44" s="119" t="s">
-        <v>104</v>
-      </c>
-      <c r="G44" s="95"/>
-      <c r="H44" s="95"/>
-      <c r="I44" s="95"/>
-      <c r="J44" s="95"/>
-      <c r="K44" s="96"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="120" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" s="96"/>
+      <c r="H44" s="96"/>
+      <c r="I44" s="96"/>
+      <c r="J44" s="96"/>
+      <c r="K44" s="97"/>
     </row>
     <row r="45" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="58" t="s">
@@ -6451,18 +6451,18 @@
         <f>+Cálculos!E60</f>
         <v>106.5</v>
       </c>
-      <c r="D45" s="118" t="s">
+      <c r="D45" s="119" t="s">
         <v>70</v>
       </c>
-      <c r="E45" s="95"/>
-      <c r="F45" s="119" t="s">
-        <v>105</v>
-      </c>
-      <c r="G45" s="95"/>
-      <c r="H45" s="95"/>
-      <c r="I45" s="95"/>
-      <c r="J45" s="95"/>
-      <c r="K45" s="96"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="120" t="s">
+        <v>103</v>
+      </c>
+      <c r="G45" s="96"/>
+      <c r="H45" s="96"/>
+      <c r="I45" s="96"/>
+      <c r="J45" s="96"/>
+      <c r="K45" s="97"/>
     </row>
     <row r="46" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="64" t="s">
@@ -6472,35 +6472,35 @@
         <f>+Cálculos!E61</f>
         <v>0.99052132701421802</v>
       </c>
-      <c r="D46" s="120" t="s">
+      <c r="D46" s="121" t="s">
         <v>73</v>
       </c>
-      <c r="E46" s="92"/>
-      <c r="F46" s="126" t="s">
-        <v>112</v>
-      </c>
-      <c r="G46" s="92"/>
-      <c r="H46" s="92"/>
-      <c r="I46" s="92"/>
-      <c r="J46" s="92"/>
-      <c r="K46" s="93"/>
+      <c r="E46" s="93"/>
+      <c r="F46" s="127" t="s">
+        <v>110</v>
+      </c>
+      <c r="G46" s="93"/>
+      <c r="H46" s="93"/>
+      <c r="I46" s="93"/>
+      <c r="J46" s="93"/>
+      <c r="K46" s="94"/>
     </row>
     <row r="47" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49"/>
-      <c r="B49" s="97" t="s">
-        <v>115</v>
-      </c>
-      <c r="C49" s="98"/>
-      <c r="D49" s="98"/>
-      <c r="E49" s="98"/>
-      <c r="F49" s="98"/>
-      <c r="G49" s="98"/>
-      <c r="H49" s="98"/>
-      <c r="I49" s="98"/>
-      <c r="J49" s="98"/>
-      <c r="K49" s="99"/>
+      <c r="B49" s="98" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="99"/>
+      <c r="D49" s="99"/>
+      <c r="E49" s="99"/>
+      <c r="F49" s="99"/>
+      <c r="G49" s="99"/>
+      <c r="H49" s="99"/>
+      <c r="I49" s="99"/>
+      <c r="J49" s="99"/>
+      <c r="K49" s="100"/>
       <c r="L49" s="49"/>
       <c r="M49" s="49"/>
       <c r="N49" s="49"/>
@@ -6519,16 +6519,16 @@
     </row>
     <row r="50" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="49"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="101"/>
-      <c r="D50" s="101"/>
-      <c r="E50" s="101"/>
-      <c r="F50" s="101"/>
-      <c r="G50" s="101"/>
-      <c r="H50" s="101"/>
-      <c r="I50" s="101"/>
-      <c r="J50" s="101"/>
-      <c r="K50" s="102"/>
+      <c r="B50" s="101"/>
+      <c r="C50" s="102"/>
+      <c r="D50" s="102"/>
+      <c r="E50" s="102"/>
+      <c r="F50" s="102"/>
+      <c r="G50" s="102"/>
+      <c r="H50" s="102"/>
+      <c r="I50" s="102"/>
+      <c r="J50" s="102"/>
+      <c r="K50" s="103"/>
       <c r="L50" s="49"/>
       <c r="M50" s="49"/>
       <c r="N50" s="49"/>
@@ -6547,16 +6547,16 @@
     </row>
     <row r="51" spans="1:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="49"/>
-      <c r="B51" s="103"/>
-      <c r="C51" s="104"/>
-      <c r="D51" s="104"/>
-      <c r="E51" s="104"/>
-      <c r="F51" s="104"/>
-      <c r="G51" s="104"/>
-      <c r="H51" s="104"/>
-      <c r="I51" s="104"/>
-      <c r="J51" s="104"/>
-      <c r="K51" s="105"/>
+      <c r="B51" s="104"/>
+      <c r="C51" s="105"/>
+      <c r="D51" s="105"/>
+      <c r="E51" s="105"/>
+      <c r="F51" s="105"/>
+      <c r="G51" s="105"/>
+      <c r="H51" s="105"/>
+      <c r="I51" s="105"/>
+      <c r="J51" s="105"/>
+      <c r="K51" s="106"/>
       <c r="L51" s="49"/>
       <c r="M51" s="49"/>
       <c r="N51" s="49"/>
@@ -6603,16 +6603,16 @@
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I54" s="123"/>
-      <c r="J54" s="122"/>
-      <c r="K54" s="122"/>
+      <c r="I54" s="124"/>
+      <c r="J54" s="123"/>
+      <c r="K54" s="123"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I55" s="124" t="s">
+      <c r="I55" s="125" t="s">
         <v>75</v>
       </c>
-      <c r="J55" s="125"/>
-      <c r="K55" s="125"/>
+      <c r="J55" s="126"/>
+      <c r="K55" s="126"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>